<commit_message>
My multi-row/col soln in EDA
</commit_message>
<xml_diff>
--- a/Excel_Challenge_496 - Sum Marks.xlsx
+++ b/Excel_Challenge_496 - Sum Marks.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BA6FDEF-BC5D-415B-81FB-D5890704C59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BCEAB8-6A06-48F1-8E78-CAB857C1D480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -90,13 +113,16 @@
   </si>
   <si>
     <t>Spanish-73, English-99, French 92</t>
+  </si>
+  <si>
+    <t>Simple</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +137,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -142,10 +175,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -153,8 +187,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -610,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -711,4 +747,523 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667937DD-4C65-4B76-A497-8CAD545BDAB1}">
+  <dimension ref="A1:N39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="str" cm="1">
+        <f t="array" ref="B14:B23">UPPER(TRIM(_xlfn.DROP(_xlfn.REDUCE("",B3:B7,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,,",")))),1)))</f>
+        <v>SPANISH - 45</v>
+      </c>
+      <c r="C14" t="str" cm="1">
+        <f t="array" ref="C14:C23">_xlfn.TEXTSPLIT(_xlfn.CONCAT(_xlfn.ANCHORARRAY(B14)),,_xlfn.ANCHORARRAY(N14),TRUE)</f>
+        <v xml:space="preserve"> - 45</v>
+      </c>
+      <c r="D14" t="str" cm="1">
+        <f t="array" ref="D14:D23">_xlfn.TEXTSPLIT(_xlfn.ANCHORARRAY(B14),_xlfn.ANCHORARRAY(C14))</f>
+        <v>SPANISH</v>
+      </c>
+      <c r="E14" cm="1">
+        <f t="array" ref="E14:E23">ABS(_xlfn.ANCHORARRAY(C14)+0)</f>
+        <v>45</v>
+      </c>
+      <c r="F14" t="str" cm="1">
+        <f t="array" ref="F14:F17">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn.ANCHORARRAY(D14)))</f>
+        <v>ENGLISH</v>
+      </c>
+      <c r="G14" t="str" cm="1">
+        <f t="array" ref="G14:G17">PROPER(_xlfn.ANCHORARRAY(F14))</f>
+        <v>English</v>
+      </c>
+      <c r="H14" cm="1">
+        <f t="array" ref="H14:H17">SUMIF(_xlfn.ANCHORARRAY(D14),_xlfn.ANCHORARRAY(F14),_xlfn.ANCHORARRAY(E14))</f>
+        <v>200</v>
+      </c>
+      <c r="I14" t="b" cm="1">
+        <f t="array" ref="I14:J17">G14:H17=D3:E6</f>
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" cm="1">
+        <f t="array" ref="M14:M39">_xlfn.SEQUENCE(26,1,CODE("A"))</f>
+        <v>65</v>
+      </c>
+      <c r="N14" t="str" cm="1">
+        <f t="array" ref="N14:N39">CHAR(_xlfn.ANCHORARRAY(M14))</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <v>ENGLISH34</v>
+      </c>
+      <c r="C15" t="str">
+        <v>34</v>
+      </c>
+      <c r="D15" t="str">
+        <v>ENGLISH</v>
+      </c>
+      <c r="E15">
+        <v>34</v>
+      </c>
+      <c r="F15" t="str">
+        <v>FRENCH</v>
+      </c>
+      <c r="G15" t="str">
+        <v>French</v>
+      </c>
+      <c r="H15">
+        <v>256</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>66</v>
+      </c>
+      <c r="N15" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B16" t="str">
+        <v>FRENCH-76</v>
+      </c>
+      <c r="C16" t="str">
+        <v>-76</v>
+      </c>
+      <c r="D16" t="str">
+        <v>FRENCH</v>
+      </c>
+      <c r="E16">
+        <v>76</v>
+      </c>
+      <c r="F16" t="str">
+        <v>PORTUGUESE</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Portuguese</v>
+      </c>
+      <c r="H16">
+        <v>55</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>67</v>
+      </c>
+      <c r="N16" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B17" t="str">
+        <v>PORTUGUESE-55</v>
+      </c>
+      <c r="C17" t="str">
+        <v>-55</v>
+      </c>
+      <c r="D17" t="str">
+        <v>PORTUGUESE</v>
+      </c>
+      <c r="E17">
+        <v>55</v>
+      </c>
+      <c r="F17" t="str">
+        <v>SPANISH</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Spanish</v>
+      </c>
+      <c r="H17">
+        <v>206</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>68</v>
+      </c>
+      <c r="N17" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" t="str">
+        <v>ENGLISH - 67</v>
+      </c>
+      <c r="C18" t="str">
+        <v xml:space="preserve"> - 67</v>
+      </c>
+      <c r="D18" t="str">
+        <v>ENGLISH</v>
+      </c>
+      <c r="E18">
+        <v>67</v>
+      </c>
+      <c r="M18">
+        <v>69</v>
+      </c>
+      <c r="N18" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" t="str">
+        <v>FRENCH88</v>
+      </c>
+      <c r="C19" t="str">
+        <v>88</v>
+      </c>
+      <c r="D19" t="str">
+        <v>FRENCH</v>
+      </c>
+      <c r="E19">
+        <v>88</v>
+      </c>
+      <c r="M19">
+        <v>70</v>
+      </c>
+      <c r="N19" t="str">
+        <v>F</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <v>SPANISH 88</v>
+      </c>
+      <c r="C20" t="str">
+        <v xml:space="preserve"> 88</v>
+      </c>
+      <c r="D20" t="str">
+        <v>SPANISH</v>
+      </c>
+      <c r="E20">
+        <v>88</v>
+      </c>
+      <c r="M20">
+        <v>71</v>
+      </c>
+      <c r="N20" t="str">
+        <v>G</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" t="str">
+        <v>SPANISH-73</v>
+      </c>
+      <c r="C21" t="str">
+        <v>-73</v>
+      </c>
+      <c r="D21" t="str">
+        <v>SPANISH</v>
+      </c>
+      <c r="E21">
+        <v>73</v>
+      </c>
+      <c r="M21">
+        <v>72</v>
+      </c>
+      <c r="N21" t="str">
+        <v>H</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" t="str">
+        <v>ENGLISH-99</v>
+      </c>
+      <c r="C22" t="str">
+        <v>-99</v>
+      </c>
+      <c r="D22" t="str">
+        <v>ENGLISH</v>
+      </c>
+      <c r="E22">
+        <v>99</v>
+      </c>
+      <c r="M22">
+        <v>73</v>
+      </c>
+      <c r="N22" t="str">
+        <v>I</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B23" t="str">
+        <v>FRENCH 92</v>
+      </c>
+      <c r="C23" t="str">
+        <v xml:space="preserve"> 92</v>
+      </c>
+      <c r="D23" t="str">
+        <v>FRENCH</v>
+      </c>
+      <c r="E23">
+        <v>92</v>
+      </c>
+      <c r="M23">
+        <v>74</v>
+      </c>
+      <c r="N23" t="str">
+        <v>J</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M24">
+        <v>75</v>
+      </c>
+      <c r="N24" t="str">
+        <v>K</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M25">
+        <v>76</v>
+      </c>
+      <c r="N25" t="str">
+        <v>L</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M26">
+        <v>77</v>
+      </c>
+      <c r="N26" t="str">
+        <v>M</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M27">
+        <v>78</v>
+      </c>
+      <c r="N27" t="str">
+        <v>N</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M28">
+        <v>79</v>
+      </c>
+      <c r="N28" t="str">
+        <v>O</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M29">
+        <v>80</v>
+      </c>
+      <c r="N29" t="str">
+        <v>P</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M30">
+        <v>81</v>
+      </c>
+      <c r="N30" t="str">
+        <v>Q</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M31">
+        <v>82</v>
+      </c>
+      <c r="N31" t="str">
+        <v>R</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M32">
+        <v>83</v>
+      </c>
+      <c r="N32" t="str">
+        <v>S</v>
+      </c>
+    </row>
+    <row r="33" spans="13:14" x14ac:dyDescent="0.3">
+      <c r="M33">
+        <v>84</v>
+      </c>
+      <c r="N33" t="str">
+        <v>T</v>
+      </c>
+    </row>
+    <row r="34" spans="13:14" x14ac:dyDescent="0.3">
+      <c r="M34">
+        <v>85</v>
+      </c>
+      <c r="N34" t="str">
+        <v>U</v>
+      </c>
+    </row>
+    <row r="35" spans="13:14" x14ac:dyDescent="0.3">
+      <c r="M35">
+        <v>86</v>
+      </c>
+      <c r="N35" t="str">
+        <v>V</v>
+      </c>
+    </row>
+    <row r="36" spans="13:14" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <v>87</v>
+      </c>
+      <c r="N36" t="str">
+        <v>W</v>
+      </c>
+    </row>
+    <row r="37" spans="13:14" x14ac:dyDescent="0.3">
+      <c r="M37">
+        <v>88</v>
+      </c>
+      <c r="N37" t="str">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="38" spans="13:14" x14ac:dyDescent="0.3">
+      <c r="M38">
+        <v>89</v>
+      </c>
+      <c r="N38" t="str">
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="39" spans="13:14" x14ac:dyDescent="0.3">
+      <c r="M39">
+        <v>90</v>
+      </c>
+      <c r="N39" t="str">
+        <v>Z</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>